<commit_message>
[Bug]: Khi set mỗi temperature như này, vẫn còn vấn đề là thi thoảng bị KẾT QUẢ OUTPUT SAI KHÁC, chắc cần kiểm soát thêm tham số nào đó để kết quả cố định
    response = client.chat.completions.create(
        model="gpt-4o-mini",
        messages=api_messages,
        temperature=0,
    )
</commit_message>
<xml_diff>
--- a/6_TuningWith2Prompting/result.xlsx
+++ b/6_TuningWith2Prompting/result.xlsx
@@ -43,16 +43,16 @@
     <t>What is your name?</t>
   </si>
   <si>
-    <t>I am Cuong, your AI Assistant. How can I help you today?</t>
-  </si>
-  <si>
-    <t>Hello Cuong! I'm Minh, your AI Assistant. How can I assist you today?</t>
-  </si>
-  <si>
-    <t>Hello Minh! It seems like we have a fun mix-up here. I'm Cuong, your AI Assistant. How can I assist you today?</t>
-  </si>
-  <si>
-    <t>Hello Cuong! It looks like we’re both AI Assistants here. How can I assist you today?</t>
+    <t>I am Cuong, your AI assistant. How can I help you today?</t>
+  </si>
+  <si>
+    <t>Hello Cuong! I'm Minh, your AI assistant. How can I assist you today?</t>
+  </si>
+  <si>
+    <t>Hello Minh! It seems like there's a little mix-up, but I'm here to assist you. How can I help you today?</t>
+  </si>
+  <si>
+    <t>Thank you, Cuong! I appreciate your willingness to assist. If you have any questions or need information on a specific topic, feel free to ask!</t>
   </si>
   <si>
     <t>-------------------</t>
@@ -61,13 +61,13 @@
     <t>My name is Cuong, and I'm here to assist you! How can I help you today?</t>
   </si>
   <si>
-    <t>Hi Cuong! I'm here to help you with any questions or tasks you have. What can I assist you with today?</t>
-  </si>
-  <si>
-    <t>Hi there! It seems like you might have mixed up our roles a bit. I'm here to assist you! If you have any questions or tasks you need help with, feel free to ask. What can I do for you today?</t>
-  </si>
-  <si>
-    <t>Thank you for the clarification, Cuong! I appreciate your willingness to assist. If you have any questions or topics you'd like to discuss, feel free to let me know. How can I help you today?</t>
+    <t>Hi Cuong! I'm here to assist you as well. How can I help you today?</t>
+  </si>
+  <si>
+    <t>Hi there! I appreciate your offer to help. I'm here to provide information and answer any questions you might have. What would you like to know or discuss today?</t>
+  </si>
+  <si>
+    <t>Thank you, Cuong! I appreciate your willingness to help. If you have any questions or topics in mind, feel free to share, and I'll do my best to assist you!</t>
   </si>
   <si>
     <t>You are Cuong. You are AI Assistant</t>
@@ -462,7 +462,7 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>1.124949216842651</v>
+        <v>1.115615606307983</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -479,7 +479,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>0.7513773441314697</v>
+        <v>0.7531790733337402</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -496,7 +496,7 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>1.053507804870605</v>
+        <v>0.9417111873626709</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -513,7 +513,7 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>0.9112639427185059</v>
+        <v>1.120330810546875</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -558,7 +558,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>0.7712469100952148</v>
+        <v>0.8064866065979004</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
@@ -575,7 +575,7 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>0.8190987110137939</v>
+        <v>0.8226840496063232</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
@@ -592,7 +592,7 @@
         <v>15</v>
       </c>
       <c r="C10">
-        <v>1.235138177871704</v>
+        <v>1.499311447143555</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
@@ -609,7 +609,7 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>1.640358686447144</v>
+        <v>1.115266799926758</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
update để cố định hơn response với các tham số khác ngoài temperature=0 +++++ Consume 30 min cho phần check response này -)))
temperature=0,
  max_completion_tokens=2048,
  top_p=1,
  frequency_penalty=0,
  presence_penalty=0
</commit_message>
<xml_diff>
--- a/6_TuningWith2Prompting/result.xlsx
+++ b/6_TuningWith2Prompting/result.xlsx
@@ -52,7 +52,7 @@
     <t>Hello Minh! It seems like there's a little mix-up, but I'm here to assist you. How can I help you today?</t>
   </si>
   <si>
-    <t>Thank you, Cuong! I appreciate your willingness to assist. If you have any questions or need information on a specific topic, feel free to ask!</t>
+    <t>Thank you, Cuong! I appreciate your willingness to help. If you have any questions or need assistance with something specific, feel free to let me know!</t>
   </si>
   <si>
     <t>-------------------</t>
@@ -61,13 +61,13 @@
     <t>My name is Cuong, and I'm here to assist you! How can I help you today?</t>
   </si>
   <si>
-    <t>Hi Cuong! I'm here to assist you as well. How can I help you today?</t>
-  </si>
-  <si>
-    <t>Hi there! I appreciate your offer to help. I'm here to provide information and answer any questions you might have. What would you like to know or discuss today?</t>
-  </si>
-  <si>
-    <t>Thank you, Cuong! I appreciate your willingness to help. If you have any questions or topics in mind, feel free to share, and I'll do my best to assist you!</t>
+    <t>Hello Cuong! I'm here to assist you as well. How can I help you today?</t>
+  </si>
+  <si>
+    <t>Hello! I appreciate your offer to help. I'm here to assist you with any questions or information you need. What would you like to know or discuss today?</t>
+  </si>
+  <si>
+    <t>Thank you, Cuong! I appreciate your willingness to assist. I’m here to provide information and answer any questions you might have. Is there a specific topic or question you’d like to discuss?</t>
   </si>
   <si>
     <t>You are Cuong. You are AI Assistant</t>
@@ -462,7 +462,7 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>1.115615606307983</v>
+        <v>1.275030851364136</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -479,7 +479,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>0.7531790733337402</v>
+        <v>1.213689804077148</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -496,7 +496,7 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>0.9417111873626709</v>
+        <v>1.02789568901062</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -513,7 +513,7 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>1.120330810546875</v>
+        <v>1.816789388656616</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -558,7 +558,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>0.8064866065979004</v>
+        <v>0.7870028018951416</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
@@ -575,7 +575,7 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>0.8226840496063232</v>
+        <v>0.8151404857635498</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
@@ -592,7 +592,7 @@
         <v>15</v>
       </c>
       <c r="C10">
-        <v>1.499311447143555</v>
+        <v>1.332005023956299</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
@@ -609,7 +609,7 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>1.115266799926758</v>
+        <v>1.669925451278687</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>

</xml_diff>